<commit_message>
update weiche testcase v2.4.3 by Travis
</commit_message>
<xml_diff>
--- a/Buding_Secondary_TestCases/Coupon/布丁优惠券V3.7测试用例.xlsx
+++ b/Buding_Secondary_TestCases/Coupon/布丁优惠券V3.7测试用例.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="180" windowWidth="24240" windowHeight="13740" tabRatio="631" activeTab="3"/>
+    <workbookView xWindow="1260" yWindow="180" windowWidth="24240" windowHeight="13740" tabRatio="631" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeList" sheetId="12" r:id="rId1"/>
@@ -4464,6 +4464,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4479,38 +4512,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4521,10 +4527,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4537,12 +4543,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5258,7 +5258,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="57">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -5280,7 +5280,7 @@
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="42.75">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
@@ -5298,7 +5298,7 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="171">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -5316,7 +5316,7 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="28.5">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="57">
-      <c r="A6" s="35"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
@@ -5352,7 +5352,7 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="28.5">
-      <c r="A7" s="36"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
@@ -5518,34 +5518,34 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="66">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>693</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="47" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="22" t="s">
         <v>142</v>
       </c>
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="8"/>
       <c r="F3" s="16" t="s">
         <v>143</v>
@@ -5556,12 +5556,12 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="42.75">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="31"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="8"/>
       <c r="F4" s="16" t="s">
         <v>145</v>
@@ -5572,35 +5572,35 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="21" t="s">
         <v>147</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="22" t="s">
         <v>149</v>
       </c>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="36"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="30"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="22" t="s">
         <v>144</v>
       </c>
       <c r="H6" s="8"/>
@@ -5723,8 +5723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C75"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5769,7 +5769,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="156.75">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -5794,7 +5794,7 @@
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="228">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>638</v>
       </c>
@@ -5817,7 +5817,7 @@
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="156.75">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -5840,7 +5840,7 @@
       <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" ht="128.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
@@ -5865,14 +5865,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="114">
-      <c r="A6" s="35"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="32" t="s">
         <v>620</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="32" t="s">
         <v>619</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -5888,12 +5888,12 @@
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="57">
-      <c r="A7" s="35"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="16" t="s">
         <v>52</v>
       </c>
@@ -5907,12 +5907,12 @@
       <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="171">
-      <c r="A8" s="35"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="16" t="s">
         <v>52</v>
       </c>
@@ -5926,17 +5926,17 @@
       <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" ht="42.75">
-      <c r="A9" s="35"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="32" t="s">
         <v>621</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="32" t="s">
         <v>622</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="32" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="16" t="s">
@@ -5949,13 +5949,13 @@
       <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="57">
-      <c r="A10" s="35"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="16" t="s">
         <v>152</v>
       </c>
@@ -5966,13 +5966,13 @@
       <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" ht="57">
-      <c r="A11" s="35"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="16" t="s">
         <v>154</v>
       </c>
@@ -5983,15 +5983,15 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="57">
-      <c r="A12" s="35"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="16" t="s">
         <v>623</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="16" t="s">
         <v>156</v>
       </c>
@@ -6002,14 +6002,14 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" ht="71.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="32" t="s">
         <v>624</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="32" t="s">
         <v>625</v>
       </c>
       <c r="E13" s="16" t="s">
@@ -6025,12 +6025,12 @@
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" ht="28.5">
-      <c r="A14" s="35"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="16" t="s">
         <v>626</v>
       </c>
@@ -6044,12 +6044,12 @@
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" ht="42.75">
-      <c r="A15" s="35"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="16" t="s">
         <v>52</v>
       </c>
@@ -6063,11 +6063,11 @@
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="57">
-      <c r="A16" s="35"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="16" t="s">
         <v>411</v>
       </c>
@@ -6084,12 +6084,12 @@
       <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="142.5">
-      <c r="A17" s="35"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32" t="s">
         <v>414</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -6105,12 +6105,12 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" ht="28.5">
-      <c r="A18" s="35"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="16" t="s">
         <v>52</v>
       </c>
@@ -6124,12 +6124,12 @@
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" ht="57">
-      <c r="A19" s="35"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="33" t="s">
         <v>389</v>
       </c>
       <c r="E19" s="16" t="s">
@@ -6145,12 +6145,12 @@
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="28.5">
-      <c r="A20" s="35"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="23"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
@@ -6164,12 +6164,12 @@
       <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="28.5">
-      <c r="A21" s="35"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="23"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="16" t="s">
         <v>52</v>
       </c>
@@ -6183,12 +6183,12 @@
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" ht="28.5">
-      <c r="A22" s="35"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="23"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="16" t="s">
         <v>52</v>
       </c>
@@ -6202,12 +6202,12 @@
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" ht="28.5">
-      <c r="A23" s="35"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="23"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="16" t="s">
         <v>52</v>
       </c>
@@ -6221,12 +6221,12 @@
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" ht="28.5">
-      <c r="A24" s="35"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="23"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="16" t="s">
         <v>52</v>
       </c>
@@ -6240,12 +6240,12 @@
       <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" ht="28.5">
-      <c r="A25" s="35"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="23"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="16" t="s">
         <v>52</v>
       </c>
@@ -6259,12 +6259,12 @@
       <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9" ht="42.75">
-      <c r="A26" s="35"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="23"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="16" t="s">
         <v>626</v>
       </c>
@@ -6278,12 +6278,12 @@
       <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" ht="57">
-      <c r="A27" s="35"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="24"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="16" t="s">
         <v>626</v>
       </c>
@@ -6297,11 +6297,11 @@
       <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" ht="42.75">
-      <c r="A28" s="35"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="16" t="s">
         <v>611</v>
       </c>
@@ -6318,14 +6318,14 @@
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" ht="85.5">
-      <c r="A29" s="35"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="32" t="s">
         <v>627</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="32" t="s">
         <v>628</v>
       </c>
       <c r="E29" s="16" t="s">
@@ -6341,12 +6341,12 @@
       <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" ht="71.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="16" t="s">
         <v>52</v>
       </c>
@@ -6360,12 +6360,12 @@
       <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" ht="71.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="16" t="s">
         <v>52</v>
       </c>
@@ -6379,14 +6379,14 @@
       <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A32" s="35"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="32" t="s">
         <v>630</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="32" t="s">
         <v>629</v>
       </c>
       <c r="E32" s="16" t="s">
@@ -6402,12 +6402,12 @@
       <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" ht="114">
-      <c r="A33" s="35"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -6421,12 +6421,12 @@
       <c r="I33" s="16"/>
     </row>
     <row r="34" spans="1:9" ht="71.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="19" t="s">
         <v>639</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="16" t="s">
         <v>52</v>
       </c>
@@ -6440,12 +6440,12 @@
       <c r="I34" s="16"/>
     </row>
     <row r="35" spans="1:9" ht="28.5">
-      <c r="A35" s="35"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="19" t="s">
         <v>640</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="16" t="s">
         <v>52</v>
       </c>
@@ -6459,12 +6459,12 @@
       <c r="I35" s="16"/>
     </row>
     <row r="36" spans="1:9" ht="242.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="19" t="s">
         <v>641</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="16" t="s">
         <v>52</v>
       </c>
@@ -6478,12 +6478,12 @@
       <c r="I36" s="16"/>
     </row>
     <row r="37" spans="1:9" ht="85.5">
-      <c r="A37" s="35"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="19" t="s">
         <v>642</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="16" t="s">
         <v>52</v>
       </c>
@@ -6497,12 +6497,12 @@
       <c r="I37" s="16"/>
     </row>
     <row r="38" spans="1:9" ht="114">
-      <c r="A38" s="35"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="19" t="s">
         <v>643</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32" t="s">
         <v>181</v>
       </c>
       <c r="E38" s="16" t="s">
@@ -6518,12 +6518,12 @@
       <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" ht="114">
-      <c r="A39" s="35"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="19" t="s">
         <v>644</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="16" t="s">
         <v>52</v>
       </c>
@@ -6537,12 +6537,12 @@
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="1:9" ht="99.75">
-      <c r="A40" s="35"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="19" t="s">
         <v>645</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21" t="s">
+      <c r="C40" s="32"/>
+      <c r="D40" s="32" t="s">
         <v>186</v>
       </c>
       <c r="E40" s="16" t="s">
@@ -6558,12 +6558,12 @@
       <c r="I40" s="16"/>
     </row>
     <row r="41" spans="1:9" ht="99.75">
-      <c r="A41" s="35"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="19" t="s">
         <v>646</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="16" t="s">
         <v>52</v>
       </c>
@@ -6577,12 +6577,12 @@
       <c r="I41" s="16"/>
     </row>
     <row r="42" spans="1:9" ht="114">
-      <c r="A42" s="35"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="19" t="s">
         <v>647</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="16" t="s">
         <v>52</v>
       </c>
@@ -6596,12 +6596,12 @@
       <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" ht="85.5">
-      <c r="A43" s="35"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="19" t="s">
         <v>648</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="16" t="s">
         <v>52</v>
       </c>
@@ -6615,12 +6615,12 @@
       <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" ht="85.5">
-      <c r="A44" s="35"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="19" t="s">
         <v>649</v>
       </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="16" t="s">
         <v>52</v>
       </c>
@@ -6634,12 +6634,12 @@
       <c r="I44" s="16"/>
     </row>
     <row r="45" spans="1:9" ht="99.75">
-      <c r="A45" s="35"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="19" t="s">
         <v>650</v>
       </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="16" t="s">
         <v>52</v>
       </c>
@@ -6653,12 +6653,12 @@
       <c r="I45" s="16"/>
     </row>
     <row r="46" spans="1:9" ht="85.5">
-      <c r="A46" s="35"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="19" t="s">
         <v>651</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="16" t="s">
         <v>52</v>
       </c>
@@ -6672,12 +6672,12 @@
       <c r="I46" s="16"/>
     </row>
     <row r="47" spans="1:9" ht="85.5">
-      <c r="A47" s="35"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="19" t="s">
         <v>652</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="16" t="s">
         <v>52</v>
       </c>
@@ -6691,12 +6691,12 @@
       <c r="I47" s="16"/>
     </row>
     <row r="48" spans="1:9" ht="99.75">
-      <c r="A48" s="35"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="19" t="s">
         <v>653</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="16" t="s">
         <v>52</v>
       </c>
@@ -6710,12 +6710,12 @@
       <c r="I48" s="16"/>
     </row>
     <row r="49" spans="1:9" ht="99.75">
-      <c r="A49" s="35"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="19" t="s">
         <v>654</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="16" t="s">
         <v>52</v>
       </c>
@@ -6729,12 +6729,12 @@
       <c r="I49" s="16"/>
     </row>
     <row r="50" spans="1:9" ht="85.5">
-      <c r="A50" s="35"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="19" t="s">
         <v>655</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="16" t="s">
         <v>52</v>
       </c>
@@ -6748,12 +6748,12 @@
       <c r="I50" s="16"/>
     </row>
     <row r="51" spans="1:9" ht="99.75">
-      <c r="A51" s="35"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="19" t="s">
         <v>656</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="16" t="s">
         <v>52</v>
       </c>
@@ -6767,12 +6767,12 @@
       <c r="I51" s="16"/>
     </row>
     <row r="52" spans="1:9" ht="128.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="19" t="s">
         <v>657</v>
       </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="16" t="s">
         <v>52</v>
       </c>
@@ -6786,12 +6786,12 @@
       <c r="I52" s="16"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="35"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="19" t="s">
         <v>658</v>
       </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
       <c r="E53" s="16" t="s">
         <v>52</v>
       </c>
@@ -6805,12 +6805,12 @@
       <c r="I53" s="16"/>
     </row>
     <row r="54" spans="1:9" ht="142.5">
-      <c r="A54" s="35"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="19" t="s">
         <v>659</v>
       </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="16" t="s">
         <v>52</v>
       </c>
@@ -6824,12 +6824,12 @@
       <c r="I54" s="16"/>
     </row>
     <row r="55" spans="1:9" ht="128.25">
-      <c r="A55" s="35"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="19" t="s">
         <v>660</v>
       </c>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21" t="s">
+      <c r="C55" s="32"/>
+      <c r="D55" s="32" t="s">
         <v>214</v>
       </c>
       <c r="E55" s="16" t="s">
@@ -6845,12 +6845,12 @@
       <c r="I55" s="16"/>
     </row>
     <row r="56" spans="1:9" ht="128.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="19" t="s">
         <v>661</v>
       </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="16" t="s">
         <v>52</v>
       </c>
@@ -6864,12 +6864,12 @@
       <c r="I56" s="16"/>
     </row>
     <row r="57" spans="1:9" ht="128.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="19" t="s">
         <v>662</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="16" t="s">
         <v>52</v>
       </c>
@@ -6883,12 +6883,12 @@
       <c r="I57" s="16"/>
     </row>
     <row r="58" spans="1:9" ht="128.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="19" t="s">
         <v>663</v>
       </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
       <c r="E58" s="16" t="s">
         <v>52</v>
       </c>
@@ -6902,12 +6902,12 @@
       <c r="I58" s="16"/>
     </row>
     <row r="59" spans="1:9" ht="128.25">
-      <c r="A59" s="35"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="19" t="s">
         <v>664</v>
       </c>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="16" t="s">
         <v>52</v>
       </c>
@@ -6921,12 +6921,12 @@
       <c r="I59" s="16"/>
     </row>
     <row r="60" spans="1:9" ht="128.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="19" t="s">
         <v>665</v>
       </c>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
       <c r="E60" s="16" t="s">
         <v>52</v>
       </c>
@@ -6940,12 +6940,12 @@
       <c r="I60" s="16"/>
     </row>
     <row r="61" spans="1:9" ht="128.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="19" t="s">
         <v>666</v>
       </c>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
       <c r="E61" s="16" t="s">
         <v>52</v>
       </c>
@@ -6959,12 +6959,12 @@
       <c r="I61" s="16"/>
     </row>
     <row r="62" spans="1:9" ht="128.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="19" t="s">
         <v>667</v>
       </c>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
       <c r="E62" s="16" t="s">
         <v>52</v>
       </c>
@@ -6978,12 +6978,12 @@
       <c r="I62" s="16"/>
     </row>
     <row r="63" spans="1:9" ht="128.25">
-      <c r="A63" s="35"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="19" t="s">
         <v>668</v>
       </c>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
       <c r="E63" s="16" t="s">
         <v>52</v>
       </c>
@@ -6997,12 +6997,12 @@
       <c r="I63" s="16"/>
     </row>
     <row r="64" spans="1:9" ht="128.25">
-      <c r="A64" s="35"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="19" t="s">
         <v>669</v>
       </c>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
       <c r="E64" s="16" t="s">
         <v>52</v>
       </c>
@@ -7016,12 +7016,12 @@
       <c r="I64" s="16"/>
     </row>
     <row r="65" spans="1:9" ht="128.25">
-      <c r="A65" s="35"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="19" t="s">
         <v>670</v>
       </c>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
       <c r="E65" s="16" t="s">
         <v>52</v>
       </c>
@@ -7035,11 +7035,11 @@
       <c r="I65" s="16"/>
     </row>
     <row r="66" spans="1:9" ht="57">
-      <c r="A66" s="35"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="19" t="s">
         <v>671</v>
       </c>
-      <c r="C66" s="21"/>
+      <c r="C66" s="32"/>
       <c r="D66" s="16" t="s">
         <v>228</v>
       </c>
@@ -7056,11 +7056,11 @@
       <c r="I66" s="16"/>
     </row>
     <row r="67" spans="1:9" ht="128.25">
-      <c r="A67" s="35"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="19" t="s">
         <v>672</v>
       </c>
-      <c r="C67" s="21"/>
+      <c r="C67" s="32"/>
       <c r="D67" s="16" t="s">
         <v>231</v>
       </c>
@@ -7077,12 +7077,12 @@
       <c r="I67" s="16"/>
     </row>
     <row r="68" spans="1:9" ht="28.5">
-      <c r="A68" s="35"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="19" t="s">
         <v>673</v>
       </c>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21" t="s">
+      <c r="C68" s="32"/>
+      <c r="D68" s="32" t="s">
         <v>234</v>
       </c>
       <c r="E68" s="16" t="s">
@@ -7098,12 +7098,12 @@
       <c r="I68" s="16"/>
     </row>
     <row r="69" spans="1:9" ht="28.5">
-      <c r="A69" s="35"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="19" t="s">
         <v>674</v>
       </c>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
       <c r="E69" s="16" t="s">
         <v>52</v>
       </c>
@@ -7117,12 +7117,12 @@
       <c r="I69" s="16"/>
     </row>
     <row r="70" spans="1:9" ht="28.5">
-      <c r="A70" s="35"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="19" t="s">
         <v>675</v>
       </c>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
       <c r="E70" s="16" t="s">
         <v>52</v>
       </c>
@@ -7136,12 +7136,12 @@
       <c r="I70" s="16"/>
     </row>
     <row r="71" spans="1:9" ht="28.5">
-      <c r="A71" s="35"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="19" t="s">
         <v>676</v>
       </c>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
       <c r="E71" s="16" t="s">
         <v>52</v>
       </c>
@@ -7155,12 +7155,12 @@
       <c r="I71" s="16"/>
     </row>
     <row r="72" spans="1:9" ht="71.25">
-      <c r="A72" s="35"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="19" t="s">
         <v>677</v>
       </c>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21" t="s">
+      <c r="C72" s="32"/>
+      <c r="D72" s="32" t="s">
         <v>241</v>
       </c>
       <c r="E72" s="16" t="s">
@@ -7176,12 +7176,12 @@
       <c r="I72" s="16"/>
     </row>
     <row r="73" spans="1:9" ht="28.5">
-      <c r="A73" s="35"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="19" t="s">
         <v>678</v>
       </c>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
       <c r="E73" s="16" t="s">
         <v>52</v>
       </c>
@@ -7195,12 +7195,12 @@
       <c r="I73" s="16"/>
     </row>
     <row r="74" spans="1:9" ht="42.75">
-      <c r="A74" s="35"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="19" t="s">
         <v>679</v>
       </c>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21" t="s">
+      <c r="C74" s="32"/>
+      <c r="D74" s="32" t="s">
         <v>246</v>
       </c>
       <c r="E74" s="16" t="s">
@@ -7216,12 +7216,12 @@
       <c r="I74" s="16"/>
     </row>
     <row r="75" spans="1:9" ht="57">
-      <c r="A75" s="35"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="19" t="s">
         <v>680</v>
       </c>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="16" t="s">
         <v>52</v>
       </c>
@@ -7235,11 +7235,11 @@
       <c r="I75" s="16"/>
     </row>
     <row r="76" spans="1:9" ht="299.25">
-      <c r="A76" s="35"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="19" t="s">
         <v>681</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="32" t="s">
         <v>637</v>
       </c>
       <c r="D76" s="16" t="s">
@@ -7258,12 +7258,12 @@
       <c r="I76" s="16"/>
     </row>
     <row r="77" spans="1:9" ht="42.75">
-      <c r="A77" s="35"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="19" t="s">
         <v>682</v>
       </c>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21" t="s">
+      <c r="C77" s="32"/>
+      <c r="D77" s="32" t="s">
         <v>590</v>
       </c>
       <c r="E77" s="16" t="s">
@@ -7279,12 +7279,12 @@
       <c r="I77" s="16"/>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="35"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="19" t="s">
         <v>683</v>
       </c>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
       <c r="E78" s="16" t="s">
         <v>52</v>
       </c>
@@ -7298,11 +7298,11 @@
       <c r="I78" s="16"/>
     </row>
     <row r="79" spans="1:9" ht="99.75">
-      <c r="A79" s="35"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="19" t="s">
         <v>684</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="C79" s="32" t="s">
         <v>636</v>
       </c>
       <c r="D79" s="16" t="s">
@@ -7323,11 +7323,11 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="35"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="19" t="s">
         <v>685</v>
       </c>
-      <c r="C80" s="21"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="16" t="s">
         <v>569</v>
       </c>
@@ -7344,12 +7344,12 @@
       <c r="I80" s="16"/>
     </row>
     <row r="81" spans="1:9" ht="71.25">
-      <c r="A81" s="35"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="19" t="s">
         <v>686</v>
       </c>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21" t="s">
+      <c r="C81" s="32"/>
+      <c r="D81" s="32" t="s">
         <v>572</v>
       </c>
       <c r="E81" s="16" t="s">
@@ -7367,12 +7367,12 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="42.75">
-      <c r="A82" s="35"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="19" t="s">
         <v>687</v>
       </c>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
       <c r="E82" s="16" t="s">
         <v>52</v>
       </c>
@@ -7386,12 +7386,12 @@
       <c r="I82" s="16"/>
     </row>
     <row r="83" spans="1:9" ht="42.75">
-      <c r="A83" s="35"/>
+      <c r="A83" s="30"/>
       <c r="B83" s="19" t="s">
         <v>688</v>
       </c>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21" t="s">
+      <c r="C83" s="32"/>
+      <c r="D83" s="32" t="s">
         <v>578</v>
       </c>
       <c r="E83" s="16" t="s">
@@ -7407,12 +7407,12 @@
       <c r="I83" s="16"/>
     </row>
     <row r="84" spans="1:9" ht="99.75">
-      <c r="A84" s="35"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="19" t="s">
         <v>689</v>
       </c>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
       <c r="E84" s="16" t="s">
         <v>52</v>
       </c>
@@ -7428,11 +7428,11 @@
       </c>
     </row>
     <row r="85" spans="1:9" ht="42.75">
-      <c r="A85" s="35"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="19" t="s">
         <v>690</v>
       </c>
-      <c r="C85" s="21"/>
+      <c r="C85" s="32"/>
       <c r="D85" s="16" t="s">
         <v>584</v>
       </c>
@@ -7449,7 +7449,7 @@
       <c r="I85" s="16"/>
     </row>
     <row r="86" spans="1:9" ht="85.5">
-      <c r="A86" s="35"/>
+      <c r="A86" s="30"/>
       <c r="B86" s="19" t="s">
         <v>691</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="I86" s="16"/>
     </row>
     <row r="87" spans="1:9" ht="71.25">
-      <c r="A87" s="36"/>
+      <c r="A87" s="31"/>
       <c r="B87" s="19" t="s">
         <v>692</v>
       </c>
@@ -7496,6 +7496,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C13:C28"/>
+    <mergeCell ref="D19:D27"/>
     <mergeCell ref="A2:A87"/>
     <mergeCell ref="C32:C75"/>
     <mergeCell ref="D38:D39"/>
@@ -7507,15 +7516,6 @@
     <mergeCell ref="D32:D37"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C13:C28"/>
-    <mergeCell ref="D19:D27"/>
     <mergeCell ref="C79:C85"/>
     <mergeCell ref="D81:D82"/>
     <mergeCell ref="D83:D84"/>
@@ -7596,16 +7596,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="228" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>705</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="43" t="s">
         <v>709</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="42" t="s">
         <v>711</v>
       </c>
       <c r="E2" s="16" t="s">
@@ -7614,65 +7614,65 @@
       <c r="F2" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="39" t="s">
         <v>252</v>
       </c>
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="33">
-      <c r="A3" s="27"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="7" t="s">
         <v>694</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="33">
-      <c r="A4" s="27"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="G4" s="38"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="33">
-      <c r="A5" s="27"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="132">
-      <c r="A6" s="27"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="7" t="s">
         <v>256</v>
       </c>
@@ -7688,12 +7688,12 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="33">
-      <c r="A7" s="27"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="42" t="s">
         <v>259</v>
       </c>
       <c r="E7" s="16" t="s">
@@ -7702,82 +7702,82 @@
       <c r="F7" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="36" t="s">
         <v>261</v>
       </c>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="33">
-      <c r="A8" s="27"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="G8" s="27"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="33">
-      <c r="A9" s="27"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="33">
-      <c r="A10" s="27"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="33">
-      <c r="A11" s="27"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="66" customHeight="1">
-      <c r="A12" s="27"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="42" t="s">
         <v>266</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -7786,34 +7786,34 @@
       <c r="F12" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="36" t="s">
         <v>268</v>
       </c>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="33">
-      <c r="A13" s="27"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="G13" s="26"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="82.5" customHeight="1">
-      <c r="A14" s="27"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="42" t="s">
         <v>270</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -7822,34 +7822,34 @@
       <c r="F14" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="36" t="s">
         <v>272</v>
       </c>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="33">
-      <c r="A15" s="27"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="G15" s="26"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="66" customHeight="1">
-      <c r="A16" s="27"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="43"/>
+      <c r="D16" s="42" t="s">
         <v>274</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -7858,34 +7858,34 @@
       <c r="F16" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="36" t="s">
         <v>276</v>
       </c>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="33">
-      <c r="A17" s="27"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="38"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="33">
-      <c r="A18" s="27"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29" t="s">
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
         <v>278</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -7894,34 +7894,34 @@
       <c r="F18" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="36" t="s">
         <v>280</v>
       </c>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="33">
-      <c r="A19" s="27"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="G19" s="38"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" ht="33">
-      <c r="A20" s="27"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="42" t="s">
         <v>282</v>
       </c>
       <c r="E20" s="16" t="s">
@@ -7930,34 +7930,34 @@
       <c r="F20" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="36" t="s">
         <v>284</v>
       </c>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" ht="33">
-      <c r="A21" s="27"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42"/>
       <c r="E21" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="33">
-      <c r="A22" s="27"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="43"/>
+      <c r="D22" s="42" t="s">
         <v>286</v>
       </c>
       <c r="E22" s="16" t="s">
@@ -7966,33 +7966,33 @@
       <c r="F22" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="36" t="s">
         <v>288</v>
       </c>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="33">
-      <c r="A23" s="27"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="99">
-      <c r="A24" s="27"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="42" t="s">
         <v>710</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -8010,11 +8010,11 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" ht="33">
-      <c r="A25" s="27"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="8" t="s">
         <v>293</v>
       </c>
@@ -8030,14 +8030,14 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" ht="198" customHeight="1">
-      <c r="A26" s="27"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="42" t="s">
         <v>297</v>
       </c>
       <c r="E26" s="16" t="s">
@@ -8046,45 +8046,45 @@
       <c r="F26" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="39" t="s">
         <v>299</v>
       </c>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" ht="33">
-      <c r="A27" s="27"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="40"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" ht="33">
-      <c r="A28" s="27"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="29"/>
+      <c r="D28" s="42"/>
       <c r="E28" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="G28" s="39"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" ht="49.5">
-      <c r="A29" s="27"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="7" t="s">
         <v>40</v>
       </c>
@@ -8104,12 +8104,12 @@
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="27"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="42" t="s">
         <v>305</v>
       </c>
       <c r="E30" s="16" t="s">
@@ -8118,33 +8118,33 @@
       <c r="F30" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="36" t="s">
         <v>307</v>
       </c>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="27"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="29"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="38"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" ht="165">
-      <c r="A32" s="27"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="36" t="s">
         <v>309</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -8162,11 +8162,11 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="27"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="27"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="8" t="s">
         <v>313</v>
       </c>
@@ -8182,11 +8182,11 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" ht="33">
-      <c r="A34" s="27"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="7" t="s">
         <v>639</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="8" t="s">
         <v>316</v>
       </c>
@@ -8202,11 +8202,11 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" ht="115.5">
-      <c r="A35" s="27"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="8" t="s">
         <v>319</v>
       </c>
@@ -8222,11 +8222,11 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" ht="165">
-      <c r="A36" s="27"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="36" t="s">
         <v>322</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -8244,11 +8244,11 @@
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" ht="33">
-      <c r="A37" s="27"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="C37" s="27"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="8" t="s">
         <v>326</v>
       </c>
@@ -8264,11 +8264,11 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="27"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="7" t="s">
         <v>643</v>
       </c>
-      <c r="C38" s="27"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="8"/>
       <c r="E38" s="16" t="s">
         <v>52</v>
@@ -8280,11 +8280,11 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" ht="115.5">
-      <c r="A39" s="27"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="7" t="s">
         <v>644</v>
       </c>
-      <c r="C39" s="27"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="8" t="s">
         <v>330</v>
       </c>
@@ -8300,11 +8300,11 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" ht="115.5">
-      <c r="A40" s="27"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="C40" s="27"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="8" t="s">
         <v>333</v>
       </c>
@@ -8320,11 +8320,11 @@
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" ht="33">
-      <c r="A41" s="27"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="C41" s="26"/>
+      <c r="C41" s="38"/>
       <c r="D41" s="8"/>
       <c r="E41" s="16" t="s">
         <v>52</v>
@@ -8338,11 +8338,11 @@
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" ht="99">
-      <c r="A42" s="27"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="36" t="s">
         <v>338</v>
       </c>
       <c r="D42" s="8" t="s">
@@ -8360,11 +8360,11 @@
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" ht="33">
-      <c r="A43" s="27"/>
+      <c r="A43" s="37"/>
       <c r="B43" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="C43" s="27"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="8" t="s">
         <v>342</v>
       </c>
@@ -8374,17 +8374,17 @@
       <c r="F43" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="G43" s="25" t="s">
+      <c r="G43" s="36" t="s">
         <v>344</v>
       </c>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="27"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="7" t="s">
         <v>649</v>
       </c>
-      <c r="C44" s="26"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="8"/>
       <c r="E44" s="16" t="s">
         <v>52</v>
@@ -8392,15 +8392,15 @@
       <c r="F44" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="G44" s="26"/>
+      <c r="G44" s="38"/>
       <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:8" ht="115.5">
-      <c r="A45" s="27"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="7" t="s">
         <v>650</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="36" t="s">
         <v>346</v>
       </c>
       <c r="D45" s="8" t="s">
@@ -8418,11 +8418,11 @@
       <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" ht="66">
-      <c r="A46" s="27"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="C46" s="27"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="8" t="s">
         <v>350</v>
       </c>
@@ -8438,11 +8438,11 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" ht="49.5">
-      <c r="A47" s="27"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="7" t="s">
         <v>652</v>
       </c>
-      <c r="C47" s="27"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="8" t="s">
         <v>353</v>
       </c>
@@ -8458,11 +8458,11 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" ht="66">
-      <c r="A48" s="27"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="7" t="s">
         <v>653</v>
       </c>
-      <c r="C48" s="27"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="8" t="s">
         <v>356</v>
       </c>
@@ -8478,11 +8478,11 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" ht="33">
-      <c r="A49" s="27"/>
+      <c r="A49" s="37"/>
       <c r="B49" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="C49" s="26"/>
+      <c r="C49" s="38"/>
       <c r="D49" s="8" t="s">
         <v>359</v>
       </c>
@@ -8498,11 +8498,11 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="33">
-      <c r="A50" s="27"/>
+      <c r="A50" s="37"/>
       <c r="B50" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="36" t="s">
         <v>431</v>
       </c>
       <c r="D50" s="8" t="s">
@@ -8514,17 +8514,17 @@
       <c r="F50" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="G50" s="36" t="s">
         <v>433</v>
       </c>
       <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:8" ht="33">
-      <c r="A51" s="27"/>
+      <c r="A51" s="37"/>
       <c r="B51" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="C51" s="27"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="8"/>
       <c r="E51" s="16" t="s">
         <v>52</v>
@@ -8532,15 +8532,15 @@
       <c r="F51" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="37"/>
       <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:8" ht="33">
-      <c r="A52" s="27"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="C52" s="27"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="8"/>
       <c r="E52" s="16" t="s">
         <v>52</v>
@@ -8548,15 +8548,15 @@
       <c r="F52" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="37"/>
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" ht="33">
-      <c r="A53" s="27"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="7" t="s">
         <v>658</v>
       </c>
-      <c r="C53" s="27"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="8"/>
       <c r="E53" s="16" t="s">
         <v>52</v>
@@ -8564,15 +8564,15 @@
       <c r="F53" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="37"/>
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" ht="33">
-      <c r="A54" s="27"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="C54" s="27"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="8"/>
       <c r="E54" s="16" t="s">
         <v>52</v>
@@ -8580,15 +8580,15 @@
       <c r="F54" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="G54" s="26"/>
+      <c r="G54" s="38"/>
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" ht="33">
-      <c r="A55" s="27"/>
+      <c r="A55" s="37"/>
       <c r="B55" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="C55" s="27"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="8" t="s">
         <v>435</v>
       </c>
@@ -8598,17 +8598,17 @@
       <c r="F55" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="G55" s="25" t="s">
+      <c r="G55" s="36" t="s">
         <v>437</v>
       </c>
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" ht="33">
-      <c r="A56" s="27"/>
+      <c r="A56" s="37"/>
       <c r="B56" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="C56" s="27"/>
+      <c r="C56" s="37"/>
       <c r="D56" s="8"/>
       <c r="E56" s="16" t="s">
         <v>52</v>
@@ -8616,15 +8616,15 @@
       <c r="F56" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="G56" s="26"/>
+      <c r="G56" s="38"/>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" ht="33">
-      <c r="A57" s="27"/>
+      <c r="A57" s="37"/>
       <c r="B57" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="37"/>
       <c r="D57" s="8" t="s">
         <v>439</v>
       </c>
@@ -8634,17 +8634,17 @@
       <c r="F57" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="G57" s="25" t="s">
+      <c r="G57" s="36" t="s">
         <v>441</v>
       </c>
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8" ht="33">
-      <c r="A58" s="27"/>
+      <c r="A58" s="37"/>
       <c r="B58" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="C58" s="27"/>
+      <c r="C58" s="37"/>
       <c r="D58" s="8"/>
       <c r="E58" s="16" t="s">
         <v>52</v>
@@ -8652,15 +8652,15 @@
       <c r="F58" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="G58" s="26"/>
+      <c r="G58" s="38"/>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" ht="33">
-      <c r="A59" s="27"/>
+      <c r="A59" s="37"/>
       <c r="B59" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="C59" s="27"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="8" t="s">
         <v>443</v>
       </c>
@@ -8670,17 +8670,17 @@
       <c r="F59" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="G59" s="25" t="s">
+      <c r="G59" s="36" t="s">
         <v>444</v>
       </c>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" ht="33">
-      <c r="A60" s="27"/>
+      <c r="A60" s="37"/>
       <c r="B60" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="C60" s="27"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="8"/>
       <c r="E60" s="16" t="s">
         <v>52</v>
@@ -8688,15 +8688,15 @@
       <c r="F60" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="G60" s="26"/>
+      <c r="G60" s="38"/>
       <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" ht="33">
-      <c r="A61" s="27"/>
+      <c r="A61" s="37"/>
       <c r="B61" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="C61" s="27"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="8" t="s">
         <v>445</v>
       </c>
@@ -8706,17 +8706,17 @@
       <c r="F61" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="G61" s="25" t="s">
+      <c r="G61" s="36" t="s">
         <v>446</v>
       </c>
       <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" ht="33">
-      <c r="A62" s="27"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="C62" s="27"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="8"/>
       <c r="E62" s="16" t="s">
         <v>52</v>
@@ -8724,15 +8724,15 @@
       <c r="F62" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="G62" s="26"/>
+      <c r="G62" s="38"/>
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" ht="33">
-      <c r="A63" s="27"/>
+      <c r="A63" s="37"/>
       <c r="B63" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="C63" s="27"/>
+      <c r="C63" s="37"/>
       <c r="D63" s="8" t="s">
         <v>447</v>
       </c>
@@ -8742,17 +8742,17 @@
       <c r="F63" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="G63" s="25" t="s">
+      <c r="G63" s="36" t="s">
         <v>448</v>
       </c>
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" ht="33">
-      <c r="A64" s="27"/>
+      <c r="A64" s="37"/>
       <c r="B64" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="C64" s="27"/>
+      <c r="C64" s="37"/>
       <c r="D64" s="8"/>
       <c r="E64" s="16" t="s">
         <v>52</v>
@@ -8760,15 +8760,15 @@
       <c r="F64" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="G64" s="26"/>
+      <c r="G64" s="38"/>
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:8" ht="33">
-      <c r="A65" s="27"/>
+      <c r="A65" s="37"/>
       <c r="B65" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="C65" s="27"/>
+      <c r="C65" s="37"/>
       <c r="D65" s="8" t="s">
         <v>449</v>
       </c>
@@ -8778,17 +8778,17 @@
       <c r="F65" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="G65" s="25" t="s">
+      <c r="G65" s="36" t="s">
         <v>451</v>
       </c>
       <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8" ht="33">
-      <c r="A66" s="27"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="C66" s="26"/>
+      <c r="C66" s="38"/>
       <c r="D66" s="8"/>
       <c r="E66" s="16" t="s">
         <v>52</v>
@@ -8796,15 +8796,15 @@
       <c r="F66" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="G66" s="26"/>
+      <c r="G66" s="38"/>
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8" ht="280.5">
-      <c r="A67" s="27"/>
+      <c r="A67" s="37"/>
       <c r="B67" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="36" t="s">
         <v>453</v>
       </c>
       <c r="D67" s="8" t="s">
@@ -8822,11 +8822,11 @@
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:8" ht="66">
-      <c r="A68" s="27"/>
+      <c r="A68" s="37"/>
       <c r="B68" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="C68" s="27"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="8"/>
       <c r="E68" s="16" t="s">
         <v>52</v>
@@ -8840,18 +8840,18 @@
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" ht="198">
-      <c r="A69" s="27"/>
+      <c r="A69" s="37"/>
       <c r="B69" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="C69" s="26"/>
+      <c r="C69" s="38"/>
       <c r="D69" s="8" t="s">
         <v>459</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F69" s="40" t="s">
+      <c r="F69" s="24" t="s">
         <v>460</v>
       </c>
       <c r="G69" s="8" t="s">
@@ -8860,11 +8860,11 @@
       <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" ht="66">
-      <c r="A70" s="27"/>
+      <c r="A70" s="37"/>
       <c r="B70" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="36" t="s">
         <v>462</v>
       </c>
       <c r="D70" s="8" t="s">
@@ -8882,11 +8882,11 @@
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" ht="66">
-      <c r="A71" s="27"/>
+      <c r="A71" s="37"/>
       <c r="B71" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="C71" s="27"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="8"/>
       <c r="E71" s="16" t="s">
         <v>52</v>
@@ -8900,11 +8900,11 @@
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:8" ht="33">
-      <c r="A72" s="27"/>
+      <c r="A72" s="37"/>
       <c r="B72" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="C72" s="27"/>
+      <c r="C72" s="37"/>
       <c r="D72" s="8"/>
       <c r="E72" s="16" t="s">
         <v>52</v>
@@ -8918,11 +8918,11 @@
       <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:8" ht="33">
-      <c r="A73" s="27"/>
+      <c r="A73" s="37"/>
       <c r="B73" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="C73" s="27"/>
+      <c r="C73" s="37"/>
       <c r="D73" s="8"/>
       <c r="E73" s="16" t="s">
         <v>52</v>
@@ -8936,11 +8936,11 @@
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:8" ht="33">
-      <c r="A74" s="27"/>
+      <c r="A74" s="37"/>
       <c r="B74" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="C74" s="27"/>
+      <c r="C74" s="37"/>
       <c r="D74" s="8"/>
       <c r="E74" s="16" t="s">
         <v>52</v>
@@ -8954,11 +8954,11 @@
       <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:8" ht="33">
-      <c r="A75" s="27"/>
+      <c r="A75" s="37"/>
       <c r="B75" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="C75" s="27"/>
+      <c r="C75" s="37"/>
       <c r="D75" s="8"/>
       <c r="E75" s="16" t="s">
         <v>52</v>
@@ -8972,18 +8972,18 @@
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:8" ht="231">
-      <c r="A76" s="27"/>
+      <c r="A76" s="37"/>
       <c r="B76" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="C76" s="27"/>
+      <c r="C76" s="37"/>
       <c r="D76" s="8" t="s">
         <v>475</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F76" s="40" t="s">
+      <c r="F76" s="24" t="s">
         <v>476</v>
       </c>
       <c r="G76" s="8" t="s">
@@ -8992,11 +8992,11 @@
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8" ht="115.5">
-      <c r="A77" s="27"/>
+      <c r="A77" s="37"/>
       <c r="B77" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="C77" s="27"/>
+      <c r="C77" s="37"/>
       <c r="D77" s="8" t="s">
         <v>478</v>
       </c>
@@ -9012,11 +9012,11 @@
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8" ht="33">
-      <c r="A78" s="27"/>
+      <c r="A78" s="37"/>
       <c r="B78" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="C78" s="26"/>
+      <c r="C78" s="38"/>
       <c r="D78" s="8" t="s">
         <v>481</v>
       </c>
@@ -9032,11 +9032,11 @@
       <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="27"/>
+      <c r="A79" s="37"/>
       <c r="B79" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="C79" s="25" t="s">
+      <c r="C79" s="36" t="s">
         <v>484</v>
       </c>
       <c r="D79" s="8" t="s">
@@ -9054,11 +9054,11 @@
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" ht="82.5">
-      <c r="A80" s="27"/>
+      <c r="A80" s="37"/>
       <c r="B80" s="7" t="s">
         <v>685</v>
       </c>
-      <c r="C80" s="27"/>
+      <c r="C80" s="37"/>
       <c r="D80" s="8" t="s">
         <v>488</v>
       </c>
@@ -9074,11 +9074,11 @@
       <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8" ht="99">
-      <c r="A81" s="27"/>
+      <c r="A81" s="37"/>
       <c r="B81" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="C81" s="27"/>
+      <c r="C81" s="37"/>
       <c r="D81" s="8" t="s">
         <v>491</v>
       </c>
@@ -9094,11 +9094,11 @@
       <c r="H81" s="8"/>
     </row>
     <row r="82" spans="1:8" ht="115.5">
-      <c r="A82" s="27"/>
+      <c r="A82" s="37"/>
       <c r="B82" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="C82" s="26"/>
+      <c r="C82" s="38"/>
       <c r="D82" s="8" t="s">
         <v>494</v>
       </c>
@@ -9114,11 +9114,11 @@
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" ht="132">
-      <c r="A83" s="27"/>
+      <c r="A83" s="37"/>
       <c r="B83" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="C83" s="25" t="s">
+      <c r="C83" s="36" t="s">
         <v>497</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -9130,17 +9130,17 @@
       <c r="F83" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="G83" s="40" t="s">
+      <c r="G83" s="24" t="s">
         <v>500</v>
       </c>
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="1:8" ht="66">
-      <c r="A84" s="27"/>
+      <c r="A84" s="37"/>
       <c r="B84" s="7" t="s">
         <v>689</v>
       </c>
-      <c r="C84" s="27"/>
+      <c r="C84" s="37"/>
       <c r="D84" s="8" t="s">
         <v>463</v>
       </c>
@@ -9156,11 +9156,11 @@
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8" ht="66">
-      <c r="A85" s="27"/>
+      <c r="A85" s="37"/>
       <c r="B85" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="C85" s="27"/>
+      <c r="C85" s="37"/>
       <c r="D85" s="8"/>
       <c r="E85" s="16" t="s">
         <v>52</v>
@@ -9174,11 +9174,11 @@
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="1:8" ht="49.5">
-      <c r="A86" s="27"/>
+      <c r="A86" s="37"/>
       <c r="B86" s="7" t="s">
         <v>691</v>
       </c>
-      <c r="C86" s="27"/>
+      <c r="C86" s="37"/>
       <c r="D86" s="8"/>
       <c r="E86" s="16" t="s">
         <v>52</v>
@@ -9192,11 +9192,11 @@
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="1:8" ht="49.5">
-      <c r="A87" s="27"/>
+      <c r="A87" s="37"/>
       <c r="B87" s="7" t="s">
         <v>692</v>
       </c>
-      <c r="C87" s="27"/>
+      <c r="C87" s="37"/>
       <c r="D87" s="8"/>
       <c r="E87" s="16" t="s">
         <v>52</v>
@@ -9210,11 +9210,11 @@
       <c r="H87" s="8"/>
     </row>
     <row r="88" spans="1:8" ht="49.5">
-      <c r="A88" s="27"/>
+      <c r="A88" s="37"/>
       <c r="B88" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="C88" s="27"/>
+      <c r="C88" s="37"/>
       <c r="D88" s="8"/>
       <c r="E88" s="16" t="s">
         <v>52</v>
@@ -9228,11 +9228,11 @@
       <c r="H88" s="8"/>
     </row>
     <row r="89" spans="1:8" ht="49.5">
-      <c r="A89" s="27"/>
+      <c r="A89" s="37"/>
       <c r="B89" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="C89" s="26"/>
+      <c r="C89" s="38"/>
       <c r="D89" s="8"/>
       <c r="E89" s="16" t="s">
         <v>52</v>
@@ -9246,11 +9246,11 @@
       <c r="H89" s="8"/>
     </row>
     <row r="90" spans="1:8" ht="181.5">
-      <c r="A90" s="27"/>
+      <c r="A90" s="37"/>
       <c r="B90" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="C90" s="25" t="s">
+      <c r="C90" s="36" t="s">
         <v>510</v>
       </c>
       <c r="D90" s="8" t="s">
@@ -9262,37 +9262,37 @@
       <c r="F90" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="G90" s="40" t="s">
+      <c r="G90" s="24" t="s">
         <v>513</v>
       </c>
       <c r="H90" s="8"/>
     </row>
     <row r="91" spans="1:8" ht="198">
-      <c r="A91" s="27"/>
+      <c r="A91" s="37"/>
       <c r="B91" s="7" t="s">
         <v>698</v>
       </c>
-      <c r="C91" s="27"/>
+      <c r="C91" s="37"/>
       <c r="D91" s="8" t="s">
         <v>514</v>
       </c>
       <c r="E91" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F91" s="40" t="s">
+      <c r="F91" s="24" t="s">
         <v>515</v>
       </c>
-      <c r="G91" s="40" t="s">
+      <c r="G91" s="24" t="s">
         <v>516</v>
       </c>
       <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" ht="115.5">
-      <c r="A92" s="27"/>
+      <c r="A92" s="37"/>
       <c r="B92" s="7" t="s">
         <v>699</v>
       </c>
-      <c r="C92" s="26"/>
+      <c r="C92" s="38"/>
       <c r="D92" s="8" t="s">
         <v>517</v>
       </c>
@@ -9308,11 +9308,11 @@
       <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:8" ht="148.5">
-      <c r="A93" s="27"/>
+      <c r="A93" s="37"/>
       <c r="B93" s="7" t="s">
         <v>700</v>
       </c>
-      <c r="C93" s="25" t="s">
+      <c r="C93" s="36" t="s">
         <v>520</v>
       </c>
       <c r="D93" s="8" t="s">
@@ -9330,11 +9330,11 @@
       <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8" ht="66">
-      <c r="A94" s="27"/>
+      <c r="A94" s="37"/>
       <c r="B94" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="C94" s="27"/>
+      <c r="C94" s="37"/>
       <c r="D94" s="8" t="s">
         <v>524</v>
       </c>
@@ -9350,11 +9350,11 @@
       <c r="H94" s="8"/>
     </row>
     <row r="95" spans="1:8" ht="66">
-      <c r="A95" s="27"/>
+      <c r="A95" s="37"/>
       <c r="B95" s="7" t="s">
         <v>702</v>
       </c>
-      <c r="C95" s="27"/>
+      <c r="C95" s="37"/>
       <c r="D95" s="8" t="s">
         <v>527</v>
       </c>
@@ -9370,11 +9370,11 @@
       <c r="H95" s="8"/>
     </row>
     <row r="96" spans="1:8" ht="82.5">
-      <c r="A96" s="27"/>
+      <c r="A96" s="37"/>
       <c r="B96" s="7" t="s">
         <v>703</v>
       </c>
-      <c r="C96" s="27"/>
+      <c r="C96" s="37"/>
       <c r="D96" s="8" t="s">
         <v>530</v>
       </c>
@@ -9390,11 +9390,11 @@
       <c r="H96" s="8"/>
     </row>
     <row r="97" spans="1:8" ht="132">
-      <c r="A97" s="26"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="7" t="s">
         <v>704</v>
       </c>
-      <c r="C97" s="26"/>
+      <c r="C97" s="38"/>
       <c r="D97" s="8" t="s">
         <v>533</v>
       </c>
@@ -9411,6 +9411,36 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C2:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G50:G54"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="G65:G66"/>
     <mergeCell ref="C90:C92"/>
     <mergeCell ref="C93:C97"/>
     <mergeCell ref="A2:A97"/>
@@ -9423,36 +9453,6 @@
     <mergeCell ref="C36:C41"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="C45:C49"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G50:G54"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C2:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576 G1 G24:G26 G29:G1048576">
@@ -9480,7 +9480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -9523,13 +9523,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="185.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>693</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="44" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -9547,11 +9547,11 @@
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="57">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="16" t="s">
         <v>75</v>
       </c>
@@ -9567,15 +9567,15 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="42.75">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="33" t="s">
         <v>713</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -9587,13 +9587,13 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="42.75">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="16" t="s">
         <v>81</v>
       </c>
@@ -9603,13 +9603,13 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="42.75">
-      <c r="A6" s="35"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="16" t="s">
         <v>83</v>
       </c>
@@ -9619,14 +9619,14 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="28.5">
-      <c r="A7" s="35"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="33" t="s">
         <v>536</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="33" t="s">
         <v>537</v>
       </c>
       <c r="E7" s="16" t="s">
@@ -9641,12 +9641,12 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="42.75">
-      <c r="A8" s="35"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="16" t="s">
         <v>626</v>
       </c>
@@ -9659,12 +9659,12 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="42.75">
-      <c r="A9" s="35"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="16" t="s">
         <v>626</v>
       </c>
@@ -9677,12 +9677,12 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A10" s="35"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="33" t="s">
         <v>543</v>
       </c>
       <c r="E10" s="16" t="s">
@@ -9691,50 +9691,50 @@
       <c r="F10" s="16" t="s">
         <v>544</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="33" t="s">
         <v>545</v>
       </c>
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="28.5">
-      <c r="A11" s="35"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="28.5">
-      <c r="A12" s="35"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>547</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="42.75">
-      <c r="A13" s="35"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="16" t="s">
         <v>626</v>
       </c>
@@ -9747,45 +9747,45 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="42.75">
-      <c r="A14" s="35"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="33" t="s">
         <v>542</v>
       </c>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="42.75">
-      <c r="A15" s="35"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="G15" s="24"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="42.75">
-      <c r="A16" s="36"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="16" t="s">
         <v>552</v>
       </c>
@@ -9897,7 +9897,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -9939,22 +9939,22 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="57">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="47" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="32" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -9963,33 +9963,33 @@
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="57">
-      <c r="A3" s="23"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="42.75">
-      <c r="A4" s="23"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="47" t="s">
         <v>715</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="47" t="s">
         <v>784</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="32" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -10001,13 +10001,13 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="42.75">
-      <c r="A5" s="23"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="16" t="s">
         <v>716</v>
       </c>
@@ -10017,20 +10017,20 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="28.5">
-      <c r="A6" s="23"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="47" t="s">
         <v>718</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="26" t="s">
         <v>719</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>720</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="32" t="s">
         <v>721</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -10039,54 +10039,54 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="199.5">
-      <c r="A7" s="23"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="45" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="26" t="s">
         <v>723</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>724</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="16" t="s">
         <v>787</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="99.75">
-      <c r="A8" s="23"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="45" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="26" t="s">
         <v>725</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>726</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="16" t="s">
         <v>788</v>
       </c>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="57">
-      <c r="A9" s="23"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="47" t="s">
         <v>727</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>728</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="32" t="s">
         <v>729</v>
       </c>
       <c r="G9" s="16" t="s">
@@ -10095,28 +10095,28 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="57">
-      <c r="A10" s="23"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="16" t="s">
         <v>731</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="16" t="s">
         <v>789</v>
       </c>
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="85.5">
-      <c r="A11" s="23"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="45" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="26" t="s">
         <v>732</v>
       </c>
       <c r="E11" s="16" t="s">
@@ -10131,33 +10131,33 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="66" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47" t="s">
         <v>736</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="32" t="s">
         <v>737</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>738</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="27" t="s">
         <v>739</v>
       </c>
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="85.5">
-      <c r="A13" s="23"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="16" t="s">
         <v>740</v>
       </c>
@@ -10167,31 +10167,31 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="66" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="32" t="s">
         <v>741</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>742</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="27" t="s">
         <v>743</v>
       </c>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="85.5">
-      <c r="A15" s="23"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="16" t="s">
         <v>744</v>
       </c>
@@ -10201,20 +10201,20 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="128.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="47" t="s">
         <v>745</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="26" t="s">
         <v>746</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="32" t="s">
         <v>747</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="32" t="s">
         <v>792</v>
       </c>
       <c r="G16" s="16" t="s">
@@ -10223,127 +10223,127 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="156.75">
-      <c r="A17" s="23"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="45" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="26" t="s">
         <v>748</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="16" t="s">
         <v>794</v>
       </c>
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="156.75">
-      <c r="A18" s="23"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="45" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="26" t="s">
         <v>749</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>750</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="16" t="s">
         <v>795</v>
       </c>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="115.5" customHeight="1">
-      <c r="A19" s="23"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31" t="s">
+      <c r="C19" s="47"/>
+      <c r="D19" s="47" t="s">
         <v>751</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>752</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21" t="s">
+      <c r="F19" s="32"/>
+      <c r="G19" s="32" t="s">
         <v>796</v>
       </c>
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="28.5">
-      <c r="A20" s="23"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="16" t="s">
         <v>753</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="164.25" customHeight="1">
-      <c r="A21" s="23"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="16" t="s">
         <v>754</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="142.5">
-      <c r="A22" s="23"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="47"/>
+      <c r="D22" s="47" t="s">
         <v>755</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="33" t="s">
         <v>756</v>
       </c>
-      <c r="F22" s="21"/>
+      <c r="F22" s="32"/>
       <c r="G22" s="20" t="s">
         <v>797</v>
       </c>
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="128.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="20" t="s">
         <v>798</v>
       </c>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="71.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="45" t="s">
+      <c r="C24" s="47"/>
+      <c r="D24" s="26" t="s">
         <v>757</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="20" t="s">
         <v>758</v>
       </c>
@@ -10353,12 +10353,12 @@
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" ht="57">
-      <c r="A25" s="23"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="45" t="s">
+      <c r="C25" s="47"/>
+      <c r="D25" s="26" t="s">
         <v>760</v>
       </c>
       <c r="E25" s="16" t="s">
@@ -10373,7 +10373,7 @@
       <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="82.5" customHeight="1">
-      <c r="A26" s="23"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="19" t="s">
         <v>37</v>
       </c>
@@ -10395,20 +10395,20 @@
       <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" ht="28.5">
-      <c r="A27" s="23"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="32" t="s">
         <v>768</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="32" t="s">
         <v>769</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>770</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="32" t="s">
         <v>771</v>
       </c>
       <c r="G27" s="16" t="s">
@@ -10417,27 +10417,27 @@
       <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="28.5">
-      <c r="A28" s="23"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="16" t="s">
         <v>773</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="16" t="s">
         <v>800</v>
       </c>
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="28.5">
-      <c r="A29" s="23"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="33" t="s">
         <v>774</v>
       </c>
       <c r="D29" s="16" t="s">
@@ -10455,11 +10455,11 @@
       <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="42.75">
-      <c r="A30" s="23"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="16" t="s">
         <v>776</v>
       </c>
@@ -10475,15 +10475,15 @@
       <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8" ht="28.5">
-      <c r="A31" s="23"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="22" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="33" t="s">
         <v>777</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="33" t="s">
         <v>778</v>
       </c>
       <c r="F31" s="16" t="s">
@@ -10495,13 +10495,13 @@
       <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="28.5">
-      <c r="A32" s="23"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="16" t="s">
         <v>808</v>
       </c>
@@ -10511,11 +10511,11 @@
       <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="28.5">
-      <c r="A33" s="24"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="24"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="16" t="s">
         <v>781</v>
       </c>
@@ -10532,13 +10532,13 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="A2:A33"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C6:C15"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="G19:G21"/>
@@ -10552,13 +10552,13 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
@@ -10635,7 +10635,7 @@
       <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="71.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>810</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -10656,7 +10656,7 @@
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="99.75">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
@@ -10675,7 +10675,7 @@
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="71.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -10696,7 +10696,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="57">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
@@ -10715,7 +10715,7 @@
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="28.5">
-      <c r="A6" s="35"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
@@ -10734,7 +10734,7 @@
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="57">
-      <c r="A7" s="35"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
@@ -10755,7 +10755,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="71.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
@@ -10774,7 +10774,7 @@
       <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" ht="28.5">
-      <c r="A9" s="35"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="19" t="s">
         <v>20</v>
       </c>
@@ -10793,12 +10793,12 @@
       <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="28.5">
-      <c r="A10" s="35"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="19"/>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="32" t="s">
         <v>392</v>
       </c>
       <c r="E10" s="16"/>
@@ -10812,12 +10812,12 @@
       <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" ht="57">
-      <c r="A11" s="35"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
         <v>395</v>
@@ -10829,7 +10829,7 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="28.5">
-      <c r="A12" s="35"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
@@ -10848,12 +10848,12 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" ht="28.5">
-      <c r="A13" s="35"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="19"/>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="32" t="s">
         <v>399</v>
       </c>
       <c r="E13" s="16"/>
@@ -10867,12 +10867,12 @@
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="35"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="19"/>
-      <c r="D14" s="21"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16" t="s">
         <v>402</v>
@@ -10884,12 +10884,12 @@
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" ht="85.5">
-      <c r="A15" s="35"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="19"/>
-      <c r="D15" s="21"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16" t="s">
         <v>404</v>
@@ -10901,12 +10901,12 @@
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="35"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="19"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16" t="s">
         <v>406</v>
@@ -10918,7 +10918,7 @@
       <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="71.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="19" t="s">
         <v>28</v>
       </c>
@@ -10937,7 +10937,7 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" ht="99.75">
-      <c r="A18" s="35"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
@@ -10958,7 +10958,7 @@
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" ht="99.75">
-      <c r="A19" s="35"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="19" t="s">
         <v>30</v>
       </c>
@@ -10977,7 +10977,7 @@
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="71.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="19" t="s">
         <v>31</v>
       </c>
@@ -10998,14 +10998,14 @@
       <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="57">
-      <c r="A21" s="35"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="32" t="s">
         <v>560</v>
       </c>
       <c r="E21" s="16"/>
@@ -11019,14 +11019,14 @@
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" ht="57">
-      <c r="A22" s="36"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
         <v>466</v>
@@ -11082,10 +11082,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11154,13 +11154,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="33" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>693</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="44" t="s">
         <v>130</v>
       </c>
       <c r="D2" s="19" t="s">
@@ -11178,11 +11178,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5">
-      <c r="A3" s="23"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="16" t="s">
         <v>134</v>
       </c>
@@ -11198,7 +11198,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="42.75">
-      <c r="A4" s="24"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="19" t="s">
         <v>811</v>
       </c>
@@ -11221,11 +11221,11 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="15"/>
-      <c r="E5" s="47"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="15"/>
-      <c r="E6" s="47"/>
+      <c r="E6" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11234,10 +11234,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G7:G1048576 G1:H1 H5:H1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11341,12 +11341,12 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="3"/>
-      <c r="E5" s="41"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="3"/>
-      <c r="E6" s="41"/>
+      <c r="E6" s="25"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8">
@@ -11436,10 +11436,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G7:G1048576 G1:H1 H3 H5:H1048576 G4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11502,7 +11502,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="128.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="29" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -11524,7 +11524,7 @@
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="42.75">
-      <c r="A3" s="35"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="19" t="s">
         <v>694</v>
       </c>
@@ -11544,7 +11544,7 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="28.5">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -11564,7 +11564,7 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="57">
-      <c r="A5" s="35"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
@@ -11584,7 +11584,7 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="42.75">
-      <c r="A6" s="36"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
@@ -11693,10 +11693,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:H1 G7:H1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>